<commit_message>
Code for OSLMF for CapyMOA
</commit_message>
<xml_diff>
--- a/Result/OSLMF_Cap modificated/OSLMF_Cap modification comments.xlsx
+++ b/Result/OSLMF_Cap modificated/OSLMF_Cap modification comments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024-2025\M2 DS\Data Stream Processing\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024-2025\M2 DS\Data Stream Processing\project\OSLMF_for_CapyMOA\Result\OSLMF_Cap modificated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF60605-2D13-41B5-A3E8-E43AB6CD96FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F11F0E6-A6CC-4938-BC1C-D770689A26BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSLMF_Cap" sheetId="1" r:id="rId1"/>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>